<commit_message>
edited colors and names in config
</commit_message>
<xml_diff>
--- a/data/config.xlsx
+++ b/data/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ppeng.com\pzdata\docs\Project Resources\Ag Water\apps\aewsd_frick_unit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868D3CC5-548B-472C-821E-93DD3AC4622F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92036B94-4A5A-47EB-B39C-E95EA89D27AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="layers" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2888" uniqueCount="1139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2888" uniqueCount="1140">
   <si>
     <t>Name</t>
   </si>
@@ -3453,7 +3453,10 @@
     <t>#504099</t>
   </si>
   <si>
-    <t>Frick Unit Pipeline</t>
+    <t>Panama Unit Pipeline</t>
+  </si>
+  <si>
+    <t>#A2678A</t>
   </si>
 </sst>
 </file>
@@ -3852,14 +3855,14 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -4011,7 +4014,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>1139</v>
       </c>
       <c r="D6" s="1">
         <v>4</v>
@@ -4179,7 +4182,7 @@
         <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
updated app notes and data
</commit_message>
<xml_diff>
--- a/data/config.xlsx
+++ b/data/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ppeng.com\pzdata\docs\Project Resources\Ag Water\apps\aewsd_frick_unit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1A730D-86A5-45C7-B0D0-C3B87244D852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98194792-B4FB-414C-8F4A-96D764C34301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2915" uniqueCount="1150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2920" uniqueCount="1151">
   <si>
     <t>Name</t>
   </si>
@@ -3487,6 +3487,9 @@
   </si>
   <si>
     <t>display</t>
+  </si>
+  <si>
+    <t>\\ppeng.com\pzdata\clients\Arvin-Edison WSD-1215\121523003-Frick Unit Pipeline\400 GIS\Feature\Facilities\proposed_turnout_2023_10.shp</t>
   </si>
 </sst>
 </file>
@@ -3601,8 +3604,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{13AE2A8C-08DE-40F4-A2E7-494D02A4EEA7}" name="Table1" displayName="Table1" ref="A1:K23" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K23" xr:uid="{13AE2A8C-08DE-40F4-A2E7-494D02A4EEA7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{13AE2A8C-08DE-40F4-A2E7-494D02A4EEA7}" name="Table1" displayName="Table1" ref="A1:K24" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K24" xr:uid="{13AE2A8C-08DE-40F4-A2E7-494D02A4EEA7}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{ECDAEBCA-0BC9-4D6F-9D67-ED2F186EF0F7}" name="Name" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{750F9F45-74DA-4191-9FDD-C80D49E99883}" name="shape_type" dataDxfId="9"/>
@@ -3885,10 +3888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4137,9 +4140,6 @@
       <c r="J8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="1" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -4561,6 +4561,36 @@
         <v>1144</v>
       </c>
       <c r="K23" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="1">
+        <v>30</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="1" t="str">
+        <f t="shared" ref="G24" si="1">IF(AND(ISBLANK(H24),ISBLANK(I24)),"gdf",IF(ISBLANK(H24),"gdb","shp"))</f>
+        <v>shp</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>1150</v>
+      </c>
+      <c r="K24" s="1" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated with ROW and others
</commit_message>
<xml_diff>
--- a/data/config.xlsx
+++ b/data/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Arvin-Edison WSD-1215\121523003-Frick Unit Pipeline\400 GIS\Scripts\aewsd_frick_unit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432781C8-9C33-4E1F-89F8-A04772D46B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A91F45-8A60-4C42-9380-6B229CC84586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="210" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2920" uniqueCount="1151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2928" uniqueCount="1156">
   <si>
     <t>Name</t>
   </si>
@@ -3491,6 +3491,21 @@
   </si>
   <si>
     <t>G:\Arvin-Edison WSD-1215\121523003-Frick Unit Pipeline\400 GIS\Scripts\aewsd_frick_unit\data\TWSC_2023</t>
+  </si>
+  <si>
+    <t>\\ppeng.com\pzdata\clients\Arvin-Edison WSD-1215\121523003-Frick Unit Pipeline\300 CAD\320 References\Sites_Ref\2024-0115 Pipeline Eastments.shp</t>
+  </si>
+  <si>
+    <t>Pipeline ESMT</t>
+  </si>
+  <si>
+    <t>SL,PL,R-W</t>
+  </si>
+  <si>
+    <t>\\ppeng.com\pzdata\clients\Arvin-Edison WSD-1215\121523003-Frick Unit Pipeline\300 CAD\320 References\Sites_Ref\2024-0115 Pipeline SL-PL-RW.shp</t>
+  </si>
+  <si>
+    <t>#864AF9</t>
   </si>
 </sst>
 </file>
@@ -3615,8 +3630,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{13AE2A8C-08DE-40F4-A2E7-494D02A4EEA7}" name="Table1" displayName="Table1" ref="A1:K24" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K24" xr:uid="{13AE2A8C-08DE-40F4-A2E7-494D02A4EEA7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{13AE2A8C-08DE-40F4-A2E7-494D02A4EEA7}" name="Table1" displayName="Table1" ref="A1:K26" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K26" xr:uid="{13AE2A8C-08DE-40F4-A2E7-494D02A4EEA7}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{ECDAEBCA-0BC9-4D6F-9D67-ED2F186EF0F7}" name="Name" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{750F9F45-74DA-4191-9FDD-C80D49E99883}" name="shape_type" dataDxfId="9"/>
@@ -3899,10 +3914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H6" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4606,6 +4621,60 @@
         <v>1139</v>
       </c>
       <c r="K24" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="1" t="str">
+        <f>IF(AND(ISBLANK(H25),ISBLANK(I25)),"gdf",IF(ISBLANK(H25),"gdb","shp"))</f>
+        <v>shp</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>1151</v>
+      </c>
+      <c r="K25" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="1" t="str">
+        <f>IF(AND(ISBLANK(H26),ISBLANK(I26)),"gdf",IF(ISBLANK(H26),"gdb","shp"))</f>
+        <v>shp</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>1154</v>
+      </c>
+      <c r="K26" s="1" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated with new files
</commit_message>
<xml_diff>
--- a/data/config.xlsx
+++ b/data/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Arvin-Edison WSD-1215\121523003-Frick Unit Pipeline\400 GIS\Scripts\aewsd_frick_unit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85B5FEB-397B-42AE-8013-D12DF4C2A3BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED613AB9-C81B-4999-BB85-866AB847CAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="210" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2928" uniqueCount="1156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2932" uniqueCount="1157">
   <si>
     <t>Name</t>
   </si>
@@ -3493,9 +3493,6 @@
     <t>G:\Arvin-Edison WSD-1215\121523003-Frick Unit Pipeline\400 GIS\Scripts\aewsd_frick_unit\data\TWSC_2023</t>
   </si>
   <si>
-    <t>\\ppeng.com\pzdata\clients\Arvin-Edison WSD-1215\121523003-Frick Unit Pipeline\300 CAD\320 References\Sites_Ref\2024-0115 Pipeline Eastments.shp</t>
-  </si>
-  <si>
     <t>Pipeline ESMT</t>
   </si>
   <si>
@@ -3506,6 +3503,12 @@
   </si>
   <si>
     <t>#FF00FF</t>
+  </si>
+  <si>
+    <t>\\ppeng.com\pzdata\clients\Arvin-Edison WSD-1215\121523003-Frick Unit Pipeline\300 CAD\320 References\Sites_Ref\2024-0117 Shapefiles\2024-0117 Pipeline ESMT.shp</t>
+  </si>
+  <si>
+    <t>\\ppeng.com\pzdata\clients\Arvin-Edison WSD-1215\121523003-Frick Unit Pipeline\300 CAD\320 References\Sites_Ref\2024-0117 Shapefiles\2024-0117 Total Area.shp</t>
   </si>
 </sst>
 </file>
@@ -3637,8 +3640,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{13AE2A8C-08DE-40F4-A2E7-494D02A4EEA7}" name="Table1" displayName="Table1" ref="A1:K26" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K26" xr:uid="{13AE2A8C-08DE-40F4-A2E7-494D02A4EEA7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{13AE2A8C-08DE-40F4-A2E7-494D02A4EEA7}" name="Table1" displayName="Table1" ref="A1:K27" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K27" xr:uid="{13AE2A8C-08DE-40F4-A2E7-494D02A4EEA7}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{ECDAEBCA-0BC9-4D6F-9D67-ED2F186EF0F7}" name="Name" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{750F9F45-74DA-4191-9FDD-C80D49E99883}" name="shape_type" dataDxfId="9"/>
@@ -3921,10 +3924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4567,9 +4570,6 @@
       <c r="H22" s="2" t="s">
         <v>1134</v>
       </c>
-      <c r="K22" s="1" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="23" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -4601,12 +4601,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>12</v>
@@ -4622,7 +4622,7 @@
         <v>shp</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>1151</v>
+        <v>1155</v>
       </c>
       <c r="K24" s="1" t="b">
         <v>1</v>
@@ -4630,13 +4630,13 @@
     </row>
     <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="D25" s="1">
         <v>2</v>
@@ -4649,10 +4649,7 @@
         <v>shp</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>1154</v>
-      </c>
-      <c r="K25" s="1" t="b">
-        <v>1</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -4682,6 +4679,33 @@
         <v>1140</v>
       </c>
       <c r="K26" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="1">
+        <v>4</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="G27" s="1" t="str">
+        <f>IF(AND(ISBLANK(H27),ISBLANK(I27)),"gdf",IF(ISBLANK(H27),"gdb","shp"))</f>
+        <v>shp</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>1156</v>
+      </c>
+      <c r="K27" s="1" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated to add isolation valves
</commit_message>
<xml_diff>
--- a/data/config.xlsx
+++ b/data/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Arvin-Edison WSD-1215\121523003-Frick Unit Pipeline\400 GIS\Scripts\aewsd_frick_unit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A70444-9496-4C83-A222-B9F9476E1DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1A6386-5B34-4874-9B6D-5C45AF732B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="210" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Layers" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2971" uniqueCount="1168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2971" uniqueCount="1167">
   <si>
     <t>Name</t>
   </si>
@@ -3485,9 +3485,6 @@
     <t>Pipeline ESMT</t>
   </si>
   <si>
-    <t>SL,PL,R-W</t>
-  </si>
-  <si>
     <t>#FF00FF</t>
   </si>
   <si>
@@ -3542,7 +3539,7 @@
     <t>NAME</t>
   </si>
   <si>
-    <t>\\ppeng.com\pzdata\clients\Arvin-Edison WSD-1215\121523003-Frick Unit Pipeline\300 CAD\320 References\Sites_Ref\OMIT\2024-0115 Pipeline SL-PL-RW.shp</t>
+    <t>Isolation Valves</t>
   </si>
 </sst>
 </file>
@@ -4018,8 +4015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4031,7 +4028,7 @@
     <col min="5" max="5" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="102" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="54.140625" style="1" bestFit="1" customWidth="1"/>
@@ -4049,7 +4046,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -4070,7 +4067,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>46</v>
@@ -4082,19 +4079,19 @@
         <v>18</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>1150</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>1151</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>1152</v>
       </c>
       <c r="Q1" s="1"/>
     </row>
@@ -4122,7 +4119,7 @@
         <v>3</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="I2" s="1" t="str">
         <f>IF(AND(ISBLANK(J2),ISBLANK(K2)),"gdf",IF(ISBLANK(J2),"gdb","shp"))</f>
@@ -4157,7 +4154,7 @@
         <v>3</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>49</v>
@@ -4890,17 +4887,17 @@
         <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="I23" s="1" t="str">
         <f t="shared" ref="I23" si="1">IF(AND(ISBLANK(J23),ISBLANK(K23)),"gdf",IF(ISBLANK(J23),"gdb","shp"))</f>
         <v>shp</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="N23" s="1" t="b">
         <v>1</v>
@@ -4934,14 +4931,14 @@
         <v>0.5</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="I24" s="1" t="str">
         <f>IF(AND(ISBLANK(J24),ISBLANK(K24)),"gdf",IF(ISBLANK(J24),"gdb","shp"))</f>
         <v>shp</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="O24" s="1" t="b">
         <v>1</v>
@@ -4957,29 +4954,29 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>1148</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>1149</v>
-      </c>
       <c r="E25" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F25" s="1">
         <v>0.2</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>1167</v>
+        <v>1163</v>
       </c>
       <c r="I25" s="1" t="str">
         <f>IF(AND(ISBLANK(J25),ISBLANK(K25)),"gdf",IF(ISBLANK(J25),"gdb","shp"))</f>
         <v>shp</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="Q25" s="1"/>
     </row>
@@ -5004,17 +5001,17 @@
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="I26" s="1" t="str">
         <f>IF(AND(ISBLANK(J26),ISBLANK(#REF!)),"gdf",IF(ISBLANK(J26),"gdb","shp"))</f>
         <v>shp</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="O26" s="1" t="b">
         <v>1</v>
@@ -5045,14 +5042,14 @@
         <v>0.7</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="I27" s="1" t="str">
         <f>IF(AND(ISBLANK(J27),ISBLANK(K27)),"gdf",IF(ISBLANK(J27),"gdb","shp"))</f>
         <v>shp</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="N27" s="1" t="b">
         <v>1</v>
@@ -5087,7 +5084,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5100,16 +5097,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="D1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5359,8 +5356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42DE6D4D-6F98-4C87-927B-967B3053D1D4}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5373,16 +5370,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="D1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5396,11 +5393,11 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B3" t="str">
         <f>_xlfn.XLOOKUP(simple[[#This Row],[id]],Table1[id],Table1[Name])</f>
-        <v>Proposed Turnout</v>
+        <v>Isolation Valves</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -5427,23 +5424,17 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B6" t="str">
         <f>_xlfn.XLOOKUP(simple[[#This Row],[id]],Table1[id],Table1[Name])</f>
-        <v>APNs</v>
-      </c>
-      <c r="D6" t="b">
-        <v>1</v>
+        <v>Proposed Turnout</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>26</v>
-      </c>
-      <c r="B7" t="str">
+      <c r="B7" t="e">
         <f>_xlfn.XLOOKUP(simple[[#This Row],[id]],Table1[id],Table1[Name])</f>
-        <v>Frick Unit Service Area</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5465,15 +5456,24 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="e">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="str">
         <f>_xlfn.XLOOKUP(simple[[#This Row],[id]],Table1[id],Table1[Name])</f>
-        <v>#N/A</v>
+        <v>APNs</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" t="e">
+      <c r="A12">
+        <v>26</v>
+      </c>
+      <c r="B12" t="str">
         <f>_xlfn.XLOOKUP(simple[[#This Row],[id]],Table1[id],Table1[Name])</f>
-        <v>#N/A</v>
+        <v>Frick Unit Service Area</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>